<commit_message>
fix profile/example id & fix cs supportedProfile ed69deab4839cd511ef3bf4c2bcd41ad1d0bf459
</commit_message>
<xml_diff>
--- a/315-flux---mise-a-jour-des-requêtes-de-flux-pour-intégrer-les-nouvelles-rc/ig/StructureDefinition-tddui-bundle.xlsx
+++ b/315-flux---mise-a-jour-des-requêtes-de-flux-pour-intégrer-les-nouvelles-rc/ig/StructureDefinition-tddui-bundle.xlsx
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-07-30T15:05:09+00:00</t>
+    <t>2025-07-30T15:46:36+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -1110,7 +1110,7 @@
     <t>Bundle.entry:DUIOrganization.resource</t>
   </si>
   <si>
-    <t xml:space="preserve">Organization {https://interop.esante.gouv.fr/ig/fhir/tddui/StructureDefinition/tddui-Organization}
+    <t xml:space="preserve">Organization {https://interop.esante.gouv.fr/ig/fhir/tddui/StructureDefinition/tddui-organization}
 </t>
   </si>
   <si>
@@ -1232,7 +1232,7 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">Encounter {https://interop.esante.gouv.fr/ig/fhir/tddui/StructureDefinition/tddui-Encounter-sejour}
+    <t xml:space="preserve">Encounter {https://interop.esante.gouv.fr/ig/fhir/tddui/StructureDefinition/tddui-encounter-sejour}
 </t>
   </si>
   <si>
@@ -1660,7 +1660,7 @@
     <col min="8" max="8" width="13.953125" customWidth="true" bestFit="true"/>
     <col min="9" max="9" width="11.3671875" customWidth="true" bestFit="true"/>
     <col min="10" max="10" width="20.703125" customWidth="true" bestFit="true"/>
-    <col min="11" max="11" width="78.359375" customWidth="true" bestFit="true"/>
+    <col min="11" max="11" width="78.33203125" customWidth="true" bestFit="true"/>
     <col min="12" max="12" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="13" max="13" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="14" max="14" width="100.703125" customWidth="true" bestFit="true"/>

</xml_diff>